<commit_message>
add testcase for zss447, also refine testcase
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/api/impl/book/447-dateFormatDisplay.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/api/impl/book/447-dateFormatDisplay.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="45" windowWidth="19395" windowHeight="7830"/>
@@ -11,27 +11,50 @@
     <sheet name="工作表2" sheetId="2" r:id="rId2"/>
     <sheet name="工作表3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>&lt;=m/d/yyyy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;=yyyy/m/d, depends on locale</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;=No Format Configuration, depends on locale</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;=m/d/yy, doesn't support yet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="m/d/yyyy"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="新細明體"/>
-      <family val="2"/>
+      <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="新細明體"/>
-      <family val="2"/>
+      <family val="1"/>
       <charset val="136"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -56,29 +79,30 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="30" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -152,7 +176,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -187,7 +210,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -363,19 +385,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="26.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1">
         <v>41632</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>41632</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2">
+        <v>41632</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3">
+        <v>41632</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -386,12 +438,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -399,12 +451,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>